<commit_message>
Fixed encoding/decoding of html code.
</commit_message>
<xml_diff>
--- a/src/main/resources/test.xlsx
+++ b/src/main/resources/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="6">
   <si>
     <t>Hi there</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>&amp;#123;&amp;#55;</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>

</xml_diff>